<commit_message>
Added Firmware described in the guides
</commit_message>
<xml_diff>
--- a/MOTOR DRIVE/FindYourFirmwarePackage.xlsx
+++ b/MOTOR DRIVE/FindYourFirmwarePackage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Dati\Training\Lab Tests\EPC-Reference-Designs-Firmware\MOTOR DRIVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19B8DD3-FC5F-4510-AD0F-4806027AD3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCFE549-D73E-477E-A12B-5EDE6D9FF7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>EPC9146 Rev2_1</t>
   </si>
   <si>
-    <t>Firmware subdirectory</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -88,13 +85,16 @@
   </si>
   <si>
     <t>sample-mb-33ep256mc506-mclv2.X-Dummy_9145_14A_3A_1_0mohm_1_3krpm_100kHz_50ns_210806</t>
+  </si>
+  <si>
+    <t>Firmware subdirectory zip file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +106,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,10 +136,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -142,8 +151,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -491,7 +504,7 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,187 +534,203 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>17</v>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:G11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BCEDDAEE-B643-4137-9C56-AD1F92172297}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{FC631A6B-18F2-4FC6-B23E-151658C5EE25}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{1E66E152-F585-4E77-9C13-37CC0B18E950}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{5EB2B5E8-766A-480A-AFAE-8BDA91780A10}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{20F6CD97-BDF0-4606-A7FF-4662B3295A34}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{5B0A7B11-91FC-4953-B693-3301DF344DC3}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{0BFCDF95-DDFC-4B5C-AAF7-D8E947021878}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{07B4F7C5-966F-4F74-919D-832EAE41E1A2}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{9D2CA421-B757-4CF1-A6D3-05BF8567E0E1}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{415A0EAC-71E7-4940-9EB2-E053A4705BE9}"/>
+    <hyperlink ref="C2" r:id="rId11" xr:uid="{FB5F9C21-1D8F-4082-83BF-D5D6B806913D}"/>
+    <hyperlink ref="C8:C11" r:id="rId12" display="EPC9147A" xr:uid="{9821E3CC-A36B-4B51-B0BE-EE8E64822A4E}"/>
+    <hyperlink ref="C3" r:id="rId13" xr:uid="{471D0131-16F3-46BB-BFBE-139008DC861B}"/>
+    <hyperlink ref="C4:C7" r:id="rId14" display="EPC9147C" xr:uid="{DFAF747B-3896-4D28-9AF6-A69166E52EFD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId15"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added hyperlink to specific directories. Added detailed guides
</commit_message>
<xml_diff>
--- a/MOTOR DRIVE/FindYourFirmwarePackage.xlsx
+++ b/MOTOR DRIVE/FindYourFirmwarePackage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Dati\Training\Lab Tests\EPC-Reference-Designs-Firmware\MOTOR DRIVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCFE549-D73E-477E-A12B-5EDE6D9FF7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543D811E-16B9-4E42-80C7-B3F621FFD00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="-13530" windowWidth="20730" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorDriveFirmware" sheetId="1" r:id="rId1"/>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -554,7 +554,7 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -571,7 +571,7 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -588,7 +588,7 @@
       <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -605,7 +605,7 @@
       <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -622,7 +622,7 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -639,7 +639,7 @@
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -656,7 +656,7 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -673,7 +673,7 @@
       <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -690,7 +690,7 @@
       <c r="E10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -707,7 +707,7 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -728,9 +728,15 @@
     <hyperlink ref="C8:C11" r:id="rId12" display="EPC9147A" xr:uid="{9821E3CC-A36B-4B51-B0BE-EE8E64822A4E}"/>
     <hyperlink ref="C3" r:id="rId13" xr:uid="{471D0131-16F3-46BB-BFBE-139008DC861B}"/>
     <hyperlink ref="C4:C7" r:id="rId14" display="EPC9147C" xr:uid="{DFAF747B-3896-4D28-9AF6-A69166E52EFD}"/>
+    <hyperlink ref="F2" r:id="rId15" xr:uid="{91EB144F-0260-48C7-9D1D-398913684794}"/>
+    <hyperlink ref="F3" r:id="rId16" xr:uid="{7E61FCF6-041B-4BA7-B1A4-4EFA62AD09C6}"/>
+    <hyperlink ref="F4" r:id="rId17" xr:uid="{3482489D-BDFE-499E-8198-67E7461526FA}"/>
+    <hyperlink ref="F5:F7" r:id="rId18" display="G431-EPC9145-DummyNema34_50k_100n" xr:uid="{1D5F1907-FC5B-4D36-BF95-61139CE66F0C}"/>
+    <hyperlink ref="F8" r:id="rId19" xr:uid="{1F9A0E6D-F48D-4481-93E5-F580146FBD1D}"/>
+    <hyperlink ref="F9:F11" r:id="rId20" display="sample-mb-33ep256mc506-mclv2.X-Dummy_9145_14A_3A_1_0mohm_1_3krpm_100kHz_50ns_210806" xr:uid="{A15B4D2F-2A06-49BB-BF46-21E9AD1A6E67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId15"/>
-  <drawing r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId21"/>
+  <drawing r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Excel file directory
</commit_message>
<xml_diff>
--- a/MOTOR DRIVE/FindYourFirmwarePackage.xlsx
+++ b/MOTOR DRIVE/FindYourFirmwarePackage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Dati\Training\Lab Tests\EPC-Reference-Designs-Firmware\MOTOR DRIVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD077E0B-29C1-42B2-82C7-3C58422A0881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B99157-672F-4BD5-AF10-82F44B21452C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18540" yWindow="-13560" windowWidth="29025" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="23">
   <si>
     <t>Controller Board</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>G431-EPC9176_1_0-DummyNema34_50k_100n</t>
+  </si>
+  <si>
+    <t>sample-mb-33ep256mc506-mclv2.X-Dummy_9176_14A_3A_1_0mohm_1_3krpm_100kHz_50ns_230125</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H12"/>
+  <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -732,6 +735,23 @@
       </c>
       <c r="F12" s="4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -760,9 +780,12 @@
     <hyperlink ref="D8" r:id="rId21" xr:uid="{804EB349-FC97-4BB8-9A20-6A0DB7457927}"/>
     <hyperlink ref="C8" r:id="rId22" xr:uid="{38B4B5FD-9682-4098-8A34-DB1B1D92F0F4}"/>
     <hyperlink ref="F8" r:id="rId23" xr:uid="{654754A0-4F4F-4B1A-8DC6-1B14774F8253}"/>
+    <hyperlink ref="C13" r:id="rId24" xr:uid="{19EB9D35-B38B-4CAC-B2EA-35187A5AB7DC}"/>
+    <hyperlink ref="F13" r:id="rId25" xr:uid="{21A6D8A9-8864-4DA5-982F-93AF1CF03FC0}"/>
+    <hyperlink ref="D13" r:id="rId26" xr:uid="{FCA8D7CD-4EBA-4A1F-92B2-66ACD035D0FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId24"/>
-  <drawing r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId27"/>
+  <drawing r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added EPC9186 ST firmware
Added EPC9186 ST firmware for Teknic motor. it works at 24V and at 36V DcBus
</commit_message>
<xml_diff>
--- a/MOTOR DRIVE/FindYourFirmwarePackage.xlsx
+++ b/MOTOR DRIVE/FindYourFirmwarePackage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Dati\Training\Lab Tests\EPC-Reference-Designs-Firmware\MOTOR DRIVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C475081-C3FE-434D-8012-6E5352D6C724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3508D751-A3FB-4860-B78A-995BCFBE03B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4920" yWindow="-16320" windowWidth="38940" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="MotorDriveFirmware" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MotorDriveFirmware!$B$1:$G$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MotorDriveFirmware!$B$1:$G$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="28">
   <si>
     <t>Controller Board</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>InstaSPIN_F2806xM_UNIVERSAL</t>
+  </si>
+  <si>
+    <t>EPC9186 Rev1_0</t>
+  </si>
+  <si>
+    <t>G431-EPC9186_1_0-DummyNema34_50k_100n</t>
   </si>
 </sst>
 </file>
@@ -519,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H19"/>
+  <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -679,20 +685,20 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
-        <v>9</v>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
@@ -703,7 +709,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -720,7 +726,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -737,7 +743,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -754,30 +760,30 @@
         <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
@@ -788,7 +794,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -805,7 +811,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -822,7 +828,7 @@
         <v>23</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -839,7 +845,7 @@
         <v>23</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -856,7 +862,7 @@
         <v>23</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -865,48 +871,68 @@
         <v>25</v>
       </c>
     </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:G12" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:G13" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BCEDDAEE-B643-4137-9C56-AD1F92172297}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{FC631A6B-18F2-4FC6-B23E-151658C5EE25}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{1E66E152-F585-4E77-9C13-37CC0B18E950}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{5EB2B5E8-766A-480A-AFAE-8BDA91780A10}"/>
+    <hyperlink ref="D10" r:id="rId4" xr:uid="{5EB2B5E8-766A-480A-AFAE-8BDA91780A10}"/>
     <hyperlink ref="D5" r:id="rId5" xr:uid="{20F6CD97-BDF0-4606-A7FF-4662B3295A34}"/>
     <hyperlink ref="D6" r:id="rId6" xr:uid="{5B0A7B11-91FC-4953-B693-3301DF344DC3}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{0BFCDF95-DDFC-4B5C-AAF7-D8E947021878}"/>
-    <hyperlink ref="D11" r:id="rId8" xr:uid="{07B4F7C5-966F-4F74-919D-832EAE41E1A2}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{0BFCDF95-DDFC-4B5C-AAF7-D8E947021878}"/>
+    <hyperlink ref="D12" r:id="rId8" xr:uid="{07B4F7C5-966F-4F74-919D-832EAE41E1A2}"/>
     <hyperlink ref="D7" r:id="rId9" xr:uid="{9D2CA421-B757-4CF1-A6D3-05BF8567E0E1}"/>
-    <hyperlink ref="D12" r:id="rId10" xr:uid="{415A0EAC-71E7-4940-9EB2-E053A4705BE9}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{415A0EAC-71E7-4940-9EB2-E053A4705BE9}"/>
     <hyperlink ref="C2" r:id="rId11" xr:uid="{FB5F9C21-1D8F-4082-83BF-D5D6B806913D}"/>
-    <hyperlink ref="C9:C12" r:id="rId12" display="EPC9147A" xr:uid="{9821E3CC-A36B-4B51-B0BE-EE8E64822A4E}"/>
+    <hyperlink ref="C10:C13" r:id="rId12" display="EPC9147A" xr:uid="{9821E3CC-A36B-4B51-B0BE-EE8E64822A4E}"/>
     <hyperlink ref="C3" r:id="rId13" xr:uid="{471D0131-16F3-46BB-BFBE-139008DC861B}"/>
     <hyperlink ref="C4:C7" r:id="rId14" display="EPC9147C" xr:uid="{DFAF747B-3896-4D28-9AF6-A69166E52EFD}"/>
     <hyperlink ref="F2" r:id="rId15" xr:uid="{91EB144F-0260-48C7-9D1D-398913684794}"/>
     <hyperlink ref="F3" r:id="rId16" xr:uid="{7E61FCF6-041B-4BA7-B1A4-4EFA62AD09C6}"/>
     <hyperlink ref="F4" r:id="rId17" xr:uid="{3482489D-BDFE-499E-8198-67E7461526FA}"/>
     <hyperlink ref="F5:F7" r:id="rId18" display="G431-EPC9145-DummyNema34_50k_100n" xr:uid="{1D5F1907-FC5B-4D36-BF95-61139CE66F0C}"/>
-    <hyperlink ref="F9" r:id="rId19" xr:uid="{1F9A0E6D-F48D-4481-93E5-F580146FBD1D}"/>
-    <hyperlink ref="F10:F12" r:id="rId20" display="sample-mb-33ep256mc506-mclv2.X-Dummy_9145_14A_3A_1_0mohm_1_3krpm_100kHz_50ns_210806" xr:uid="{A15B4D2F-2A06-49BB-BF46-21E9AD1A6E67}"/>
+    <hyperlink ref="F10" r:id="rId19" xr:uid="{1F9A0E6D-F48D-4481-93E5-F580146FBD1D}"/>
+    <hyperlink ref="F11:F13" r:id="rId20" display="sample-mb-33ep256mc506-mclv2.X-Dummy_9145_14A_3A_1_0mohm_1_3krpm_100kHz_50ns_210806" xr:uid="{A15B4D2F-2A06-49BB-BF46-21E9AD1A6E67}"/>
     <hyperlink ref="D8" r:id="rId21" xr:uid="{804EB349-FC97-4BB8-9A20-6A0DB7457927}"/>
     <hyperlink ref="C8" r:id="rId22" xr:uid="{38B4B5FD-9682-4098-8A34-DB1B1D92F0F4}"/>
     <hyperlink ref="F8" r:id="rId23" xr:uid="{654754A0-4F4F-4B1A-8DC6-1B14774F8253}"/>
-    <hyperlink ref="C13" r:id="rId24" xr:uid="{19EB9D35-B38B-4CAC-B2EA-35187A5AB7DC}"/>
-    <hyperlink ref="F13" r:id="rId25" xr:uid="{21A6D8A9-8864-4DA5-982F-93AF1CF03FC0}"/>
-    <hyperlink ref="D13" r:id="rId26" xr:uid="{FCA8D7CD-4EBA-4A1F-92B2-66ACD035D0FB}"/>
-    <hyperlink ref="D14" r:id="rId27" xr:uid="{D8F5739F-3E0A-49EC-AC0E-0A3510F305A4}"/>
-    <hyperlink ref="D15" r:id="rId28" xr:uid="{00B3D0C5-E56D-4A32-B5BB-2ED009EB7738}"/>
-    <hyperlink ref="D16" r:id="rId29" xr:uid="{7EAF039D-CD52-4E1D-AAFE-C282742E8183}"/>
-    <hyperlink ref="D17" r:id="rId30" xr:uid="{BD35BD76-FCDA-4DE0-AFDD-D46C9C9C78D3}"/>
-    <hyperlink ref="D18" r:id="rId31" xr:uid="{8CA3D326-87C2-4A0A-82C1-3B799E2155F0}"/>
-    <hyperlink ref="D19" r:id="rId32" xr:uid="{A96E009C-F629-4C50-85A4-2EBB4A1CBB95}"/>
-    <hyperlink ref="C14" r:id="rId33" xr:uid="{FDCD2404-82D1-4A88-958A-14F87DE1C20C}"/>
-    <hyperlink ref="C15:C19" r:id="rId34" display="EPC9147B" xr:uid="{ECE2AE6B-856F-45FD-AA80-4F9164ADD387}"/>
-    <hyperlink ref="F14" r:id="rId35" xr:uid="{EB772C03-DC3D-40C5-9D71-F7014D1C173B}"/>
-    <hyperlink ref="F15:F19" r:id="rId36" display="InstaSPIN_F2806xM_UNIVERSAL" xr:uid="{A853EDB2-D453-44D7-9715-FFC3C5A90F9C}"/>
+    <hyperlink ref="C14" r:id="rId24" xr:uid="{19EB9D35-B38B-4CAC-B2EA-35187A5AB7DC}"/>
+    <hyperlink ref="F14" r:id="rId25" xr:uid="{21A6D8A9-8864-4DA5-982F-93AF1CF03FC0}"/>
+    <hyperlink ref="D14" r:id="rId26" xr:uid="{FCA8D7CD-4EBA-4A1F-92B2-66ACD035D0FB}"/>
+    <hyperlink ref="D15" r:id="rId27" xr:uid="{D8F5739F-3E0A-49EC-AC0E-0A3510F305A4}"/>
+    <hyperlink ref="D16" r:id="rId28" xr:uid="{00B3D0C5-E56D-4A32-B5BB-2ED009EB7738}"/>
+    <hyperlink ref="D17" r:id="rId29" xr:uid="{7EAF039D-CD52-4E1D-AAFE-C282742E8183}"/>
+    <hyperlink ref="D18" r:id="rId30" xr:uid="{BD35BD76-FCDA-4DE0-AFDD-D46C9C9C78D3}"/>
+    <hyperlink ref="D19" r:id="rId31" xr:uid="{8CA3D326-87C2-4A0A-82C1-3B799E2155F0}"/>
+    <hyperlink ref="D20" r:id="rId32" xr:uid="{A96E009C-F629-4C50-85A4-2EBB4A1CBB95}"/>
+    <hyperlink ref="C15" r:id="rId33" xr:uid="{FDCD2404-82D1-4A88-958A-14F87DE1C20C}"/>
+    <hyperlink ref="C16:C20" r:id="rId34" display="EPC9147B" xr:uid="{ECE2AE6B-856F-45FD-AA80-4F9164ADD387}"/>
+    <hyperlink ref="F15" r:id="rId35" xr:uid="{EB772C03-DC3D-40C5-9D71-F7014D1C173B}"/>
+    <hyperlink ref="F16:F20" r:id="rId36" display="InstaSPIN_F2806xM_UNIVERSAL" xr:uid="{A853EDB2-D453-44D7-9715-FFC3C5A90F9C}"/>
+    <hyperlink ref="D9" r:id="rId37" xr:uid="{9802CCE7-FFB8-4D54-B0BA-576085B5726B}"/>
+    <hyperlink ref="C9" r:id="rId38" xr:uid="{8BF48131-9DD9-4F0E-8BA5-BBA61C52B141}"/>
+    <hyperlink ref="F9" r:id="rId39" xr:uid="{3A9AA79A-B317-4906-AD97-5B01762F2D80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId37"/>
-  <drawing r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId40"/>
+  <drawing r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>